<commit_message>
Removed some temp characters
</commit_message>
<xml_diff>
--- a/Software Process Model/PetPal SPM REVISED.xlsx
+++ b/Software Process Model/PetPal SPM REVISED.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Desktop\University\Year 2\Spring\SE 216\Project\SE-216-Section-3-Group-6\Software Process Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\William\Desktop\Petpal\SE-216-Section-3-Group-6\Software Process Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351A6662-1192-4E9B-AEEC-1EC3533DB475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA30AC08-F051-4E94-ACE8-A1E0F8C704BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{DD0626E2-1333-F643-A88B-8507C5CC965E}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="21600" windowHeight="11385" xr2:uid="{DD0626E2-1333-F643-A88B-8507C5CC965E}"/>
   </bookViews>
   <sheets>
     <sheet name="ProductBackLog" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="125">
   <si>
     <t>#</t>
   </si>
@@ -550,18 +550,6 @@
     <t>Ensuring this is done early on, and making sure no laws are missed is important, as noticing a law that affects the project at a later stage can be a huge setback.</t>
   </si>
   <si>
-    <t>8!</t>
-  </si>
-  <si>
-    <t>7!</t>
-  </si>
-  <si>
-    <t>13!</t>
-  </si>
-  <si>
-    <t>14!</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">UI/UX Usability: </t>
     </r>
@@ -577,33 +565,6 @@
     </r>
   </si>
   <si>
-    <t>16!</t>
-  </si>
-  <si>
-    <t>17!</t>
-  </si>
-  <si>
-    <t>18!</t>
-  </si>
-  <si>
-    <t>3!</t>
-  </si>
-  <si>
-    <t>4!</t>
-  </si>
-  <si>
-    <t>1!</t>
-  </si>
-  <si>
-    <t>2+</t>
-  </si>
-  <si>
-    <t>5!</t>
-  </si>
-  <si>
-    <t>15+</t>
-  </si>
-  <si>
     <t>Layout Planning for Smart Feeding Stations</t>
   </si>
   <si>
@@ -634,9 +595,6 @@
     <t>04.04.2025</t>
   </si>
   <si>
-    <t>19+</t>
-  </si>
-  <si>
     <t>Implementing the Heatmap UI Within the Mobile App</t>
   </si>
   <si>
@@ -655,18 +613,9 @@
     <t xml:space="preserve">Making sure this can be pressed in a hurry is a must in order to ensure the safety of users. </t>
   </si>
   <si>
-    <t>10+</t>
-  </si>
-  <si>
     <t>Implementing Notifications</t>
   </si>
   <si>
-    <t>20+</t>
-  </si>
-  <si>
-    <t>9+</t>
-  </si>
-  <si>
     <t>Volunteers will be notified when nearby feeding stations are low on food or water.</t>
   </si>
   <si>
@@ -683,12 +632,6 @@
   </si>
   <si>
     <t>09.04.2025</t>
-  </si>
-  <si>
-    <t>12+</t>
-  </si>
-  <si>
-    <t>11+</t>
   </si>
   <si>
     <t>Ensure that the mobile app works on older versions of Android and IOS.</t>
@@ -7865,22 +7808,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07AF4077-26B8-2245-8ED1-A0CA9934B29A}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="83.3984375" customWidth="1"/>
+    <col min="2" max="2" width="83.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="92.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="92.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="52" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="53"/>
     </row>
-    <row r="2" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
@@ -7888,161 +7831,161 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
-        <v>66</v>
+    <row r="3" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12">
+        <v>1</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
-        <v>67</v>
+    <row r="4" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
+        <v>2</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
-        <v>64</v>
+    <row r="5" spans="1:2" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
+        <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
-        <v>65</v>
+    <row r="6" spans="1:2" ht="49.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
+        <v>4</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
-        <v>68</v>
+    <row r="7" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
+        <v>5</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
-        <v>57</v>
+    <row r="9" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12">
+        <v>7</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
-        <v>56</v>
+    <row r="10" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12">
+        <v>8</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="25" t="s">
-        <v>90</v>
+    <row r="11" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
+        <v>9</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="50.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="25" t="s">
-        <v>87</v>
+    <row r="12" spans="1:2" ht="50.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25">
+        <v>10</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="25" t="s">
-        <v>98</v>
+    <row r="13" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
+        <v>11</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="25" t="s">
-        <v>97</v>
+    <row r="14" spans="1:2" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
+        <v>12</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
-        <v>58</v>
+    <row r="15" spans="1:2" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12">
+        <v>13</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12" t="s">
-        <v>59</v>
+    <row r="16" spans="1:2" ht="47.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12">
+        <v>14</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
-        <v>69</v>
+    <row r="17" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="12">
+        <v>15</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="12">
+        <v>16</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
-        <v>62</v>
+    <row r="19" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="12">
+        <v>17</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
-        <v>63</v>
+    <row r="20" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="12">
+        <v>18</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="25" t="s">
-        <v>80</v>
+    <row r="21" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="25">
+        <v>19</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="25" t="s">
-        <v>89</v>
+    <row r="22" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25">
+        <v>20</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>44</v>
@@ -8065,25 +8008,25 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" customWidth="1"/>
-    <col min="2" max="2" width="22.8984375" customWidth="1"/>
-    <col min="3" max="3" width="39.19921875" customWidth="1"/>
-    <col min="4" max="4" width="22.8984375" customWidth="1"/>
-    <col min="5" max="6" width="32.59765625" customWidth="1"/>
-    <col min="7" max="7" width="15.59765625" customWidth="1"/>
-    <col min="8" max="8" width="12.59765625" customWidth="1"/>
+    <col min="1" max="1" width="3.375" customWidth="1"/>
+    <col min="2" max="2" width="22.875" customWidth="1"/>
+    <col min="3" max="3" width="39.25" customWidth="1"/>
+    <col min="4" max="4" width="22.875" customWidth="1"/>
+    <col min="5" max="6" width="32.625" customWidth="1"/>
+    <col min="7" max="7" width="15.625" customWidth="1"/>
+    <col min="8" max="8" width="12.625" customWidth="1"/>
     <col min="9" max="9" width="44" customWidth="1"/>
-    <col min="10" max="10" width="0.19921875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="24.09765625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="25.59765625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="28.3984375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="42.59765625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="3.3984375" customWidth="1"/>
+    <col min="10" max="10" width="0.25" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="24.125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="25.625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="28.375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="42.625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="3.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="27.6" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:15" ht="28.5" x14ac:dyDescent="0.4">
       <c r="B1" s="69" t="s">
         <v>2</v>
       </c>
@@ -8101,7 +8044,7 @@
       <c r="N1" s="17"/>
       <c r="O1" s="17"/>
     </row>
-    <row r="2" spans="2:15" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="33" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
         <v>3</v>
       </c>
@@ -8128,7 +8071,7 @@
       </c>
       <c r="M2" s="11"/>
     </row>
-    <row r="3" spans="2:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
         <v>51</v>
       </c>
@@ -8155,7 +8098,7 @@
       </c>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="2:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>51</v>
       </c>
@@ -8182,7 +8125,7 @@
       </c>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="2:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
         <v>51</v>
       </c>
@@ -8209,7 +8152,7 @@
       </c>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="2:15" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
         <v>52</v>
       </c>
@@ -8236,12 +8179,12 @@
       </c>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="2:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>15</v>
@@ -8259,11 +8202,11 @@
         <v>1</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="4"/>
@@ -8274,7 +8217,7 @@
       <c r="I8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="4"/>
@@ -8285,7 +8228,7 @@
       <c r="I9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="4"/>
@@ -8296,7 +8239,7 @@
       <c r="I10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="4"/>
@@ -8307,7 +8250,7 @@
       <c r="I11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="4"/>
@@ -8318,7 +8261,7 @@
       <c r="I12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="4"/>
@@ -8329,7 +8272,7 @@
       <c r="I13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="4"/>
@@ -8340,7 +8283,7 @@
       <c r="I14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="4"/>
@@ -8351,7 +8294,7 @@
       <c r="I15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="4"/>
@@ -8362,7 +8305,7 @@
       <c r="I16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="4"/>
@@ -8373,7 +8316,7 @@
       <c r="I17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="4"/>
@@ -8384,7 +8327,7 @@
       <c r="I18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="4"/>
@@ -8395,7 +8338,7 @@
       <c r="I19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="4"/>
@@ -8406,7 +8349,7 @@
       <c r="I20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="4"/>
@@ -8417,7 +8360,7 @@
       <c r="I21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="2:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" ht="18" x14ac:dyDescent="0.25">
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -8429,8 +8372,8 @@
       </c>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="2:14" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="54" t="s">
         <v>20</v>
       </c>
@@ -8447,7 +8390,7 @@
       <c r="M24" s="63"/>
       <c r="N24" s="64"/>
     </row>
-    <row r="25" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="57"/>
       <c r="C25" s="58"/>
       <c r="D25" s="59"/>
@@ -8462,7 +8405,7 @@
       <c r="M25" s="65"/>
       <c r="N25" s="66"/>
     </row>
-    <row r="26" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="57"/>
       <c r="C26" s="58"/>
       <c r="D26" s="59"/>
@@ -8477,7 +8420,7 @@
       <c r="M26" s="65"/>
       <c r="N26" s="66"/>
     </row>
-    <row r="27" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="57"/>
       <c r="C27" s="58"/>
       <c r="D27" s="59"/>
@@ -8492,7 +8435,7 @@
       <c r="M27" s="65"/>
       <c r="N27" s="66"/>
     </row>
-    <row r="28" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="57"/>
       <c r="C28" s="58"/>
       <c r="D28" s="59"/>
@@ -8507,7 +8450,7 @@
       <c r="M28" s="65"/>
       <c r="N28" s="66"/>
     </row>
-    <row r="29" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="57"/>
       <c r="C29" s="58"/>
       <c r="D29" s="59"/>
@@ -8522,7 +8465,7 @@
       <c r="M29" s="65"/>
       <c r="N29" s="66"/>
     </row>
-    <row r="30" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="57"/>
       <c r="C30" s="58"/>
       <c r="D30" s="59"/>
@@ -8537,7 +8480,7 @@
       <c r="M30" s="65"/>
       <c r="N30" s="66"/>
     </row>
-    <row r="31" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="57"/>
       <c r="C31" s="58"/>
       <c r="D31" s="59"/>
@@ -8552,7 +8495,7 @@
       <c r="M31" s="65"/>
       <c r="N31" s="66"/>
     </row>
-    <row r="32" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="57"/>
       <c r="C32" s="58"/>
       <c r="D32" s="59"/>
@@ -8567,7 +8510,7 @@
       <c r="M32" s="65"/>
       <c r="N32" s="66"/>
     </row>
-    <row r="33" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="60"/>
       <c r="C33" s="61"/>
       <c r="D33" s="62"/>
@@ -8582,7 +8525,7 @@
       <c r="M33" s="67"/>
       <c r="N33" s="68"/>
     </row>
-    <row r="34" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B24:D33"/>
@@ -8631,26 +8574,26 @@
       <selection activeCell="E24" sqref="E24:N33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" style="35" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="35.59765625" style="35" customWidth="1"/>
-    <col min="4" max="4" width="22.8984375" style="35" customWidth="1"/>
-    <col min="5" max="6" width="32.59765625" style="35" customWidth="1"/>
-    <col min="7" max="7" width="15.59765625" style="35" customWidth="1"/>
-    <col min="8" max="8" width="12.59765625" style="35" customWidth="1"/>
-    <col min="9" max="9" width="49.3984375" style="35" customWidth="1"/>
-    <col min="10" max="10" width="12.59765625" style="35" customWidth="1"/>
-    <col min="11" max="11" width="24.09765625" style="35" customWidth="1"/>
-    <col min="12" max="12" width="25.59765625" style="35" customWidth="1"/>
-    <col min="13" max="13" width="28.3984375" style="35" customWidth="1"/>
-    <col min="14" max="14" width="42.59765625" style="35" customWidth="1"/>
-    <col min="15" max="15" width="3.3984375" style="35" customWidth="1"/>
-    <col min="16" max="16384" width="8.8984375" style="35"/>
+    <col min="1" max="1" width="3.375" style="35" customWidth="1"/>
+    <col min="2" max="2" width="15.625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="35.625" style="35" customWidth="1"/>
+    <col min="4" max="4" width="22.875" style="35" customWidth="1"/>
+    <col min="5" max="6" width="32.625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="15.625" style="35" customWidth="1"/>
+    <col min="8" max="8" width="12.625" style="35" customWidth="1"/>
+    <col min="9" max="9" width="49.375" style="35" customWidth="1"/>
+    <col min="10" max="10" width="12.625" style="35" customWidth="1"/>
+    <col min="11" max="11" width="24.125" style="35" customWidth="1"/>
+    <col min="12" max="12" width="25.625" style="35" customWidth="1"/>
+    <col min="13" max="13" width="28.375" style="35" customWidth="1"/>
+    <col min="14" max="14" width="42.625" style="35" customWidth="1"/>
+    <col min="15" max="15" width="3.375" style="35" customWidth="1"/>
+    <col min="16" max="16384" width="8.875" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B1" s="85" t="s">
         <v>21</v>
       </c>
@@ -8668,7 +8611,7 @@
       <c r="N1" s="34"/>
       <c r="O1" s="34"/>
     </row>
-    <row r="2" spans="2:15" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="33" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
         <v>3</v>
       </c>
@@ -8695,12 +8638,12 @@
       </c>
       <c r="M2" s="30"/>
     </row>
-    <row r="3" spans="2:15" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>22</v>
@@ -8712,22 +8655,22 @@
         <v>26</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="H3" s="16">
         <v>3</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="M3" s="36"/>
     </row>
-    <row r="4" spans="2:15" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>22</v>
@@ -8736,25 +8679,25 @@
         <v>19</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="H4" s="16">
         <v>1</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="M4" s="36"/>
     </row>
-    <row r="5" spans="2:15" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>22</v>
@@ -8763,7 +8706,7 @@
         <v>19</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="G5" s="23" t="s">
         <v>27</v>
@@ -8772,16 +8715,16 @@
         <v>2</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="M5" s="36"/>
     </row>
-    <row r="6" spans="2:15" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>22</v>
@@ -8799,16 +8742,16 @@
         <v>1</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="M6" s="36"/>
     </row>
-    <row r="7" spans="2:15" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D7" s="28" t="s">
         <v>22</v>
@@ -8820,22 +8763,22 @@
         <v>28</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="H7" s="16">
         <v>2</v>
       </c>
       <c r="I7" s="26" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="M7" s="36"/>
     </row>
-    <row r="8" spans="2:15" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="D8" s="28" t="s">
         <v>22</v>
@@ -8844,25 +8787,25 @@
         <v>19</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="H8" s="16">
         <v>1</v>
       </c>
       <c r="I8" s="26" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="M8" s="36"/>
     </row>
-    <row r="9" spans="2:15" ht="97.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>22</v>
@@ -8871,25 +8814,25 @@
         <v>16</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="H9" s="16">
         <v>2</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="M9" s="36"/>
     </row>
-    <row r="10" spans="2:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>22</v>
@@ -8898,20 +8841,20 @@
         <v>12</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="H10" s="16">
         <v>2</v>
       </c>
       <c r="I10" s="26" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="M10" s="36"/>
     </row>
-    <row r="11" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
       <c r="D11" s="38"/>
@@ -8922,7 +8865,7 @@
       <c r="I11" s="41"/>
       <c r="M11" s="36"/>
     </row>
-    <row r="12" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="42"/>
       <c r="C12" s="42"/>
       <c r="D12" s="43"/>
@@ -8933,7 +8876,7 @@
       <c r="I12" s="36"/>
       <c r="M12" s="36"/>
     </row>
-    <row r="13" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="42"/>
       <c r="C13" s="42"/>
       <c r="D13" s="43"/>
@@ -8944,7 +8887,7 @@
       <c r="I13" s="36"/>
       <c r="M13" s="36"/>
     </row>
-    <row r="14" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="42"/>
       <c r="C14" s="42"/>
       <c r="D14" s="43"/>
@@ -8955,7 +8898,7 @@
       <c r="I14" s="36"/>
       <c r="M14" s="36"/>
     </row>
-    <row r="15" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="42"/>
       <c r="C15" s="42"/>
       <c r="D15" s="43"/>
@@ -8966,7 +8909,7 @@
       <c r="I15" s="36"/>
       <c r="M15" s="36"/>
     </row>
-    <row r="16" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="42"/>
       <c r="C16" s="42"/>
       <c r="D16" s="43"/>
@@ -8977,7 +8920,7 @@
       <c r="I16" s="36"/>
       <c r="M16" s="36"/>
     </row>
-    <row r="17" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="42"/>
       <c r="C17" s="42"/>
       <c r="D17" s="43"/>
@@ -8988,7 +8931,7 @@
       <c r="I17" s="36"/>
       <c r="M17" s="36"/>
     </row>
-    <row r="18" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="42"/>
       <c r="C18" s="42"/>
       <c r="D18" s="43"/>
@@ -8999,7 +8942,7 @@
       <c r="I18" s="36"/>
       <c r="M18" s="36"/>
     </row>
-    <row r="19" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="42"/>
       <c r="C19" s="42"/>
       <c r="D19" s="43"/>
@@ -9010,7 +8953,7 @@
       <c r="I19" s="36"/>
       <c r="M19" s="36"/>
     </row>
-    <row r="20" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="42"/>
       <c r="C20" s="42"/>
       <c r="D20" s="43"/>
@@ -9021,7 +8964,7 @@
       <c r="I20" s="36"/>
       <c r="M20" s="36"/>
     </row>
-    <row r="21" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="42"/>
       <c r="C21" s="42"/>
       <c r="D21" s="43"/>
@@ -9032,7 +8975,7 @@
       <c r="I21" s="36"/>
       <c r="M21" s="36"/>
     </row>
-    <row r="22" spans="2:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" ht="18" x14ac:dyDescent="0.25">
       <c r="B22" s="46"/>
       <c r="C22" s="46"/>
       <c r="D22" s="46"/>
@@ -9045,8 +8988,8 @@
       </c>
       <c r="I22" s="46"/>
     </row>
-    <row r="23" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="2:14" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="70" t="s">
         <v>20</v>
       </c>
@@ -9063,7 +9006,7 @@
       <c r="M24" s="79"/>
       <c r="N24" s="80"/>
     </row>
-    <row r="25" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="73"/>
       <c r="C25" s="74"/>
       <c r="D25" s="75"/>
@@ -9078,7 +9021,7 @@
       <c r="M25" s="81"/>
       <c r="N25" s="82"/>
     </row>
-    <row r="26" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="73"/>
       <c r="C26" s="74"/>
       <c r="D26" s="75"/>
@@ -9093,7 +9036,7 @@
       <c r="M26" s="81"/>
       <c r="N26" s="82"/>
     </row>
-    <row r="27" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="73"/>
       <c r="C27" s="74"/>
       <c r="D27" s="75"/>
@@ -9108,7 +9051,7 @@
       <c r="M27" s="81"/>
       <c r="N27" s="82"/>
     </row>
-    <row r="28" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="73"/>
       <c r="C28" s="74"/>
       <c r="D28" s="75"/>
@@ -9123,7 +9066,7 @@
       <c r="M28" s="81"/>
       <c r="N28" s="82"/>
     </row>
-    <row r="29" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="73"/>
       <c r="C29" s="74"/>
       <c r="D29" s="75"/>
@@ -9138,7 +9081,7 @@
       <c r="M29" s="81"/>
       <c r="N29" s="82"/>
     </row>
-    <row r="30" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="73"/>
       <c r="C30" s="74"/>
       <c r="D30" s="75"/>
@@ -9153,7 +9096,7 @@
       <c r="M30" s="81"/>
       <c r="N30" s="82"/>
     </row>
-    <row r="31" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="73"/>
       <c r="C31" s="74"/>
       <c r="D31" s="75"/>
@@ -9168,7 +9111,7 @@
       <c r="M31" s="81"/>
       <c r="N31" s="82"/>
     </row>
-    <row r="32" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="73"/>
       <c r="C32" s="74"/>
       <c r="D32" s="75"/>
@@ -9183,7 +9126,7 @@
       <c r="M32" s="81"/>
       <c r="N32" s="82"/>
     </row>
-    <row r="33" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="76"/>
       <c r="C33" s="77"/>
       <c r="D33" s="78"/>
@@ -9198,7 +9141,7 @@
       <c r="M33" s="83"/>
       <c r="N33" s="84"/>
     </row>
-    <row r="34" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B24:D33"/>
@@ -9242,30 +9185,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5817B818-790D-5D48-A09C-A0270AC402A3}">
   <dimension ref="B1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24:N33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" style="35" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="28.19921875" style="35" customWidth="1"/>
+    <col min="1" max="1" width="3.375" style="35" customWidth="1"/>
+    <col min="2" max="2" width="15.625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="28.25" style="35" customWidth="1"/>
     <col min="4" max="4" width="12" style="35" customWidth="1"/>
-    <col min="5" max="5" width="9.8984375" style="35" customWidth="1"/>
-    <col min="6" max="7" width="9.09765625" style="35" customWidth="1"/>
+    <col min="5" max="5" width="9.875" style="35" customWidth="1"/>
+    <col min="6" max="7" width="9.125" style="35" customWidth="1"/>
     <col min="8" max="8" width="10.5" style="35" customWidth="1"/>
-    <col min="9" max="9" width="49.3984375" style="35" customWidth="1"/>
-    <col min="10" max="10" width="12.59765625" style="35" customWidth="1"/>
-    <col min="11" max="11" width="24.09765625" style="35" customWidth="1"/>
-    <col min="12" max="12" width="25.59765625" style="35" customWidth="1"/>
-    <col min="13" max="13" width="28.3984375" style="35" customWidth="1"/>
-    <col min="14" max="14" width="42.59765625" style="35" customWidth="1"/>
-    <col min="15" max="15" width="3.3984375" style="35" customWidth="1"/>
-    <col min="16" max="16384" width="8.8984375" style="35"/>
+    <col min="9" max="9" width="49.375" style="35" customWidth="1"/>
+    <col min="10" max="10" width="12.625" style="35" customWidth="1"/>
+    <col min="11" max="11" width="24.125" style="35" customWidth="1"/>
+    <col min="12" max="12" width="25.625" style="35" customWidth="1"/>
+    <col min="13" max="13" width="28.375" style="35" customWidth="1"/>
+    <col min="14" max="14" width="42.625" style="35" customWidth="1"/>
+    <col min="15" max="15" width="3.375" style="35" customWidth="1"/>
+    <col min="16" max="16384" width="8.875" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B1" s="85" t="s">
         <v>23</v>
       </c>
@@ -9283,7 +9226,7 @@
       <c r="N1" s="34"/>
       <c r="O1" s="34"/>
     </row>
-    <row r="2" spans="2:15" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="33" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
         <v>3</v>
       </c>
@@ -9310,12 +9253,12 @@
       </c>
       <c r="M2" s="30"/>
     </row>
-    <row r="3" spans="2:15" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>22</v>
@@ -9324,25 +9267,25 @@
         <v>12</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="H3" s="16">
         <v>3</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="M3" s="36"/>
     </row>
-    <row r="4" spans="2:15" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>22</v>
@@ -9351,25 +9294,25 @@
         <v>16</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="H4" s="16">
         <v>1</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="M4" s="36"/>
     </row>
-    <row r="5" spans="2:15" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>22</v>
@@ -9378,25 +9321,25 @@
         <v>12</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="H5" s="16">
         <v>2</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="M5" s="36"/>
     </row>
-    <row r="6" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>22</v>
@@ -9405,22 +9348,22 @@
         <v>16</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="H6" s="16">
         <v>2</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="M6" s="36"/>
     </row>
-    <row r="7" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>25</v>
@@ -9432,20 +9375,20 @@
         <v>16</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="H7" s="16">
         <v>1</v>
       </c>
       <c r="I7" s="26" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="M7" s="36"/>
     </row>
-    <row r="8" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
         <v>51</v>
       </c>
@@ -9459,20 +9402,20 @@
         <v>16</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="H8" s="16">
         <v>1</v>
       </c>
       <c r="I8" s="26" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="M8" s="36"/>
     </row>
-    <row r="9" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="37"/>
       <c r="C9" s="37"/>
       <c r="D9" s="38"/>
@@ -9483,7 +9426,7 @@
       <c r="I9" s="41"/>
       <c r="M9" s="36"/>
     </row>
-    <row r="10" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="42"/>
       <c r="C10" s="42"/>
       <c r="D10" s="43"/>
@@ -9494,7 +9437,7 @@
       <c r="I10" s="36"/>
       <c r="M10" s="36"/>
     </row>
-    <row r="11" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="42"/>
       <c r="C11" s="42"/>
       <c r="D11" s="43"/>
@@ -9505,7 +9448,7 @@
       <c r="I11" s="36"/>
       <c r="M11" s="36"/>
     </row>
-    <row r="12" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="42"/>
       <c r="C12" s="42"/>
       <c r="D12" s="43"/>
@@ -9516,7 +9459,7 @@
       <c r="I12" s="36"/>
       <c r="M12" s="36"/>
     </row>
-    <row r="13" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="42"/>
       <c r="C13" s="42"/>
       <c r="D13" s="43"/>
@@ -9527,7 +9470,7 @@
       <c r="I13" s="36"/>
       <c r="M13" s="36"/>
     </row>
-    <row r="14" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="42"/>
       <c r="C14" s="42"/>
       <c r="D14" s="43"/>
@@ -9538,7 +9481,7 @@
       <c r="I14" s="36"/>
       <c r="M14" s="36"/>
     </row>
-    <row r="15" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="42"/>
       <c r="C15" s="42"/>
       <c r="D15" s="43"/>
@@ -9549,7 +9492,7 @@
       <c r="I15" s="36"/>
       <c r="M15" s="36"/>
     </row>
-    <row r="16" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="42"/>
       <c r="C16" s="42"/>
       <c r="D16" s="43"/>
@@ -9560,7 +9503,7 @@
       <c r="I16" s="36"/>
       <c r="M16" s="36"/>
     </row>
-    <row r="17" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="42"/>
       <c r="C17" s="42"/>
       <c r="D17" s="43"/>
@@ -9571,7 +9514,7 @@
       <c r="I17" s="36"/>
       <c r="M17" s="36"/>
     </row>
-    <row r="18" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="42"/>
       <c r="C18" s="42"/>
       <c r="D18" s="43"/>
@@ -9582,7 +9525,7 @@
       <c r="I18" s="36"/>
       <c r="M18" s="36"/>
     </row>
-    <row r="19" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="42"/>
       <c r="C19" s="42"/>
       <c r="D19" s="43"/>
@@ -9593,7 +9536,7 @@
       <c r="I19" s="36"/>
       <c r="M19" s="36"/>
     </row>
-    <row r="20" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="42"/>
       <c r="C20" s="42"/>
       <c r="D20" s="43"/>
@@ -9604,7 +9547,7 @@
       <c r="I20" s="36"/>
       <c r="M20" s="36"/>
     </row>
-    <row r="21" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="42"/>
       <c r="C21" s="42"/>
       <c r="D21" s="43"/>
@@ -9615,7 +9558,7 @@
       <c r="I21" s="36"/>
       <c r="M21" s="36"/>
     </row>
-    <row r="22" spans="2:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" ht="18" x14ac:dyDescent="0.25">
       <c r="B22" s="46"/>
       <c r="C22" s="46"/>
       <c r="D22" s="46"/>
@@ -9628,8 +9571,8 @@
       </c>
       <c r="I22" s="46"/>
     </row>
-    <row r="23" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="2:14" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="70" t="s">
         <v>20</v>
       </c>
@@ -9646,7 +9589,7 @@
       <c r="M24" s="79"/>
       <c r="N24" s="80"/>
     </row>
-    <row r="25" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="73"/>
       <c r="C25" s="74"/>
       <c r="D25" s="75"/>
@@ -9661,7 +9604,7 @@
       <c r="M25" s="81"/>
       <c r="N25" s="82"/>
     </row>
-    <row r="26" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="73"/>
       <c r="C26" s="74"/>
       <c r="D26" s="75"/>
@@ -9676,7 +9619,7 @@
       <c r="M26" s="81"/>
       <c r="N26" s="82"/>
     </row>
-    <row r="27" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="73"/>
       <c r="C27" s="74"/>
       <c r="D27" s="75"/>
@@ -9691,7 +9634,7 @@
       <c r="M27" s="81"/>
       <c r="N27" s="82"/>
     </row>
-    <row r="28" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="73"/>
       <c r="C28" s="74"/>
       <c r="D28" s="75"/>
@@ -9706,7 +9649,7 @@
       <c r="M28" s="81"/>
       <c r="N28" s="82"/>
     </row>
-    <row r="29" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="73"/>
       <c r="C29" s="74"/>
       <c r="D29" s="75"/>
@@ -9721,7 +9664,7 @@
       <c r="M29" s="81"/>
       <c r="N29" s="82"/>
     </row>
-    <row r="30" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="73"/>
       <c r="C30" s="74"/>
       <c r="D30" s="75"/>
@@ -9736,7 +9679,7 @@
       <c r="M30" s="81"/>
       <c r="N30" s="82"/>
     </row>
-    <row r="31" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="73"/>
       <c r="C31" s="74"/>
       <c r="D31" s="75"/>
@@ -9751,7 +9694,7 @@
       <c r="M31" s="81"/>
       <c r="N31" s="82"/>
     </row>
-    <row r="32" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="73"/>
       <c r="C32" s="74"/>
       <c r="D32" s="75"/>
@@ -9766,7 +9709,7 @@
       <c r="M32" s="81"/>
       <c r="N32" s="82"/>
     </row>
-    <row r="33" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="76"/>
       <c r="C33" s="77"/>
       <c r="D33" s="78"/>
@@ -9781,7 +9724,7 @@
       <c r="M33" s="83"/>
       <c r="N33" s="84"/>
     </row>
-    <row r="34" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:I1"/>
@@ -9829,27 +9772,27 @@
       <selection activeCell="E24" sqref="E24:N33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" style="35" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" style="35" customWidth="1"/>
+    <col min="1" max="1" width="3.375" style="35" customWidth="1"/>
+    <col min="2" max="2" width="15.625" style="35" customWidth="1"/>
     <col min="3" max="3" width="30.5" style="35" customWidth="1"/>
-    <col min="4" max="4" width="12.09765625" style="35" customWidth="1"/>
+    <col min="4" max="4" width="12.125" style="35" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="35" customWidth="1"/>
     <col min="6" max="6" width="9.5" style="35" customWidth="1"/>
-    <col min="7" max="7" width="9.59765625" style="35" customWidth="1"/>
-    <col min="8" max="8" width="10.59765625" style="35" customWidth="1"/>
-    <col min="9" max="9" width="49.3984375" style="35" customWidth="1"/>
-    <col min="10" max="10" width="12.59765625" style="35" customWidth="1"/>
-    <col min="11" max="11" width="24.09765625" style="35" customWidth="1"/>
-    <col min="12" max="12" width="25.59765625" style="35" customWidth="1"/>
-    <col min="13" max="13" width="28.3984375" style="35" customWidth="1"/>
-    <col min="14" max="14" width="42.59765625" style="35" customWidth="1"/>
-    <col min="15" max="15" width="3.3984375" style="35" customWidth="1"/>
-    <col min="16" max="16384" width="8.8984375" style="35"/>
+    <col min="7" max="7" width="9.625" style="35" customWidth="1"/>
+    <col min="8" max="8" width="10.625" style="35" customWidth="1"/>
+    <col min="9" max="9" width="49.375" style="35" customWidth="1"/>
+    <col min="10" max="10" width="12.625" style="35" customWidth="1"/>
+    <col min="11" max="11" width="24.125" style="35" customWidth="1"/>
+    <col min="12" max="12" width="25.625" style="35" customWidth="1"/>
+    <col min="13" max="13" width="28.375" style="35" customWidth="1"/>
+    <col min="14" max="14" width="42.625" style="35" customWidth="1"/>
+    <col min="15" max="15" width="3.375" style="35" customWidth="1"/>
+    <col min="16" max="16384" width="8.875" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B1" s="85" t="s">
         <v>24</v>
       </c>
@@ -9867,7 +9810,7 @@
       <c r="N1" s="34"/>
       <c r="O1" s="34"/>
     </row>
-    <row r="2" spans="2:15" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="33" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
         <v>3</v>
       </c>
@@ -9894,12 +9837,12 @@
       </c>
       <c r="M2" s="30"/>
     </row>
-    <row r="3" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>22</v>
@@ -9908,25 +9851,25 @@
         <v>19</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="H3" s="16">
         <v>1</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="M3" s="36"/>
     </row>
-    <row r="4" spans="2:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>22</v>
@@ -9935,25 +9878,25 @@
         <v>16</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="H4" s="16">
         <v>1</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="M4" s="36"/>
     </row>
-    <row r="5" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>22</v>
@@ -9962,25 +9905,25 @@
         <v>12</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="H5" s="16">
         <v>5</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="M5" s="36"/>
     </row>
-    <row r="6" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>22</v>
@@ -9989,25 +9932,25 @@
         <v>12</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="H6" s="16">
         <v>3</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="M6" s="36"/>
     </row>
-    <row r="7" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="D7" s="28" t="s">
         <v>22</v>
@@ -10016,25 +9959,25 @@
         <v>12</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="H7" s="16">
         <v>2</v>
       </c>
       <c r="I7" s="26" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="M7" s="36"/>
     </row>
-    <row r="8" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="D8" s="28" t="s">
         <v>22</v>
@@ -10043,25 +9986,25 @@
         <v>12</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="H8" s="16">
         <v>7</v>
       </c>
       <c r="I8" s="26" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="M8" s="36"/>
     </row>
-    <row r="9" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>22</v>
@@ -10079,16 +10022,16 @@
         <v>1</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="M9" s="36"/>
     </row>
-    <row r="10" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>22</v>
@@ -10097,20 +10040,20 @@
         <v>12</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="H10" s="16">
         <v>1</v>
       </c>
       <c r="I10" s="26" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="M10" s="36"/>
     </row>
-    <row r="11" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="47"/>
       <c r="C11" s="47"/>
       <c r="D11" s="48"/>
@@ -10121,7 +10064,7 @@
       <c r="I11" s="50"/>
       <c r="M11" s="36"/>
     </row>
-    <row r="12" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="47"/>
       <c r="C12" s="47"/>
       <c r="D12" s="48"/>
@@ -10132,7 +10075,7 @@
       <c r="I12" s="50"/>
       <c r="M12" s="36"/>
     </row>
-    <row r="13" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="47"/>
       <c r="C13" s="47"/>
       <c r="D13" s="48"/>
@@ -10143,7 +10086,7 @@
       <c r="I13" s="50"/>
       <c r="M13" s="36"/>
     </row>
-    <row r="14" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="37"/>
       <c r="C14" s="37"/>
       <c r="D14" s="38"/>
@@ -10154,7 +10097,7 @@
       <c r="I14" s="41"/>
       <c r="M14" s="36"/>
     </row>
-    <row r="15" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="42"/>
       <c r="C15" s="42"/>
       <c r="D15" s="43"/>
@@ -10165,7 +10108,7 @@
       <c r="I15" s="36"/>
       <c r="M15" s="36"/>
     </row>
-    <row r="16" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="42"/>
       <c r="C16" s="42"/>
       <c r="D16" s="43"/>
@@ -10176,7 +10119,7 @@
       <c r="I16" s="36"/>
       <c r="M16" s="36"/>
     </row>
-    <row r="17" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="42"/>
       <c r="C17" s="42"/>
       <c r="D17" s="43"/>
@@ -10187,7 +10130,7 @@
       <c r="I17" s="36"/>
       <c r="M17" s="36"/>
     </row>
-    <row r="18" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="42"/>
       <c r="C18" s="42"/>
       <c r="D18" s="43"/>
@@ -10198,7 +10141,7 @@
       <c r="I18" s="36"/>
       <c r="M18" s="36"/>
     </row>
-    <row r="19" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="42"/>
       <c r="C19" s="42"/>
       <c r="D19" s="43"/>
@@ -10209,7 +10152,7 @@
       <c r="I19" s="36"/>
       <c r="M19" s="36"/>
     </row>
-    <row r="20" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="42"/>
       <c r="C20" s="42"/>
       <c r="D20" s="43"/>
@@ -10220,7 +10163,7 @@
       <c r="I20" s="36"/>
       <c r="M20" s="36"/>
     </row>
-    <row r="21" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="42"/>
       <c r="C21" s="42"/>
       <c r="D21" s="43"/>
@@ -10231,7 +10174,7 @@
       <c r="I21" s="36"/>
       <c r="M21" s="36"/>
     </row>
-    <row r="22" spans="2:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" ht="18" x14ac:dyDescent="0.25">
       <c r="B22" s="46"/>
       <c r="C22" s="46"/>
       <c r="D22" s="46"/>
@@ -10244,8 +10187,8 @@
       </c>
       <c r="I22" s="46"/>
     </row>
-    <row r="23" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="2:14" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="70" t="s">
         <v>20</v>
       </c>
@@ -10262,7 +10205,7 @@
       <c r="M24" s="79"/>
       <c r="N24" s="80"/>
     </row>
-    <row r="25" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="73"/>
       <c r="C25" s="74"/>
       <c r="D25" s="75"/>
@@ -10277,7 +10220,7 @@
       <c r="M25" s="81"/>
       <c r="N25" s="82"/>
     </row>
-    <row r="26" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="73"/>
       <c r="C26" s="74"/>
       <c r="D26" s="75"/>
@@ -10292,7 +10235,7 @@
       <c r="M26" s="81"/>
       <c r="N26" s="82"/>
     </row>
-    <row r="27" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="73"/>
       <c r="C27" s="74"/>
       <c r="D27" s="75"/>
@@ -10307,7 +10250,7 @@
       <c r="M27" s="81"/>
       <c r="N27" s="82"/>
     </row>
-    <row r="28" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="73"/>
       <c r="C28" s="74"/>
       <c r="D28" s="75"/>
@@ -10322,7 +10265,7 @@
       <c r="M28" s="81"/>
       <c r="N28" s="82"/>
     </row>
-    <row r="29" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="73"/>
       <c r="C29" s="74"/>
       <c r="D29" s="75"/>
@@ -10337,7 +10280,7 @@
       <c r="M29" s="81"/>
       <c r="N29" s="82"/>
     </row>
-    <row r="30" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="73"/>
       <c r="C30" s="74"/>
       <c r="D30" s="75"/>
@@ -10352,7 +10295,7 @@
       <c r="M30" s="81"/>
       <c r="N30" s="82"/>
     </row>
-    <row r="31" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="73"/>
       <c r="C31" s="74"/>
       <c r="D31" s="75"/>
@@ -10367,7 +10310,7 @@
       <c r="M31" s="81"/>
       <c r="N31" s="82"/>
     </row>
-    <row r="32" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="73"/>
       <c r="C32" s="74"/>
       <c r="D32" s="75"/>
@@ -10382,7 +10325,7 @@
       <c r="M32" s="81"/>
       <c r="N32" s="82"/>
     </row>
-    <row r="33" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="76"/>
       <c r="C33" s="77"/>
       <c r="D33" s="78"/>
@@ -10397,7 +10340,7 @@
       <c r="M33" s="83"/>
       <c r="N33" s="84"/>
     </row>
-    <row r="34" spans="2:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B24:D33"/>

</xml_diff>